<commit_message>
windows hoofdstuk 4 start
</commit_message>
<xml_diff>
--- a/Windows/Individuele Documentatie/Jens/Windows PowerShell 3.0 Step by Step Cheatsheet.xlsx
+++ b/Windows/Individuele Documentatie/Jens/Windows PowerShell 3.0 Step by Step Cheatsheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="66">
   <si>
     <t>CheatSheet Windows PowerShell 3.0</t>
   </si>
@@ -208,6 +208,13 @@
   </si>
   <si>
     <t>Zet je locatie naar de certificaat PS drive</t>
+  </si>
+  <si>
+    <t>Get-Help * -Parameter computername | sort name | ft name, synopsis -auto -wrap</t>
+  </si>
+  <si>
+    <t>Dit commando levert een lijst van alle
+cmdlets die native ondersteuning voor remoting hebben</t>
   </si>
 </sst>
 </file>
@@ -266,7 +273,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -278,6 +285,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -579,16 +589,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="43" style="3" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" style="3" customWidth="1"/>
     <col min="3" max="3" width="45" style="3" customWidth="1"/>
   </cols>
   <sheetData>
@@ -847,7 +857,19 @@
         <v>63</v>
       </c>
     </row>
+    <row r="26" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" s="5"/>
+      <c r="C26" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A26:B26"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Windows hoofdstuk 5 en 6
</commit_message>
<xml_diff>
--- a/Windows/Individuele Documentatie/Jens/Windows PowerShell 3.0 Step by Step Cheatsheet.xlsx
+++ b/Windows/Individuele Documentatie/Jens/Windows PowerShell 3.0 Step by Step Cheatsheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="82">
   <si>
     <t>CheatSheet Windows PowerShell 3.0</t>
   </si>
@@ -215,6 +215,54 @@
   <si>
     <t>Dit commando levert een lijst van alle
 cmdlets die native ondersteuning voor remoting hebben</t>
+  </si>
+  <si>
+    <t>Start-Transcript</t>
+  </si>
+  <si>
+    <t>Enter-PSSession</t>
+  </si>
+  <si>
+    <t>-Computername &lt;computer&gt;</t>
+  </si>
+  <si>
+    <t>Start een eenvoudige remote acces naar de computer. De prompt zal veranderen naar de naam van de computer.</t>
+  </si>
+  <si>
+    <t>!Zeer Nuttig! Wanneer je dit commando uitvoert, zullen alle commando's die hierna worden uitgevoerd, worden lokaal opgeslagen in een tekstbestand. Opmerking: stop deze functie door gebruik te maken van het commando Stop-transcript</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invoke-Command </t>
+  </si>
+  <si>
+    <t>Als je slechts 1 commando moet uitvoeren op een remote machine, dan maak je gebruik van dit commando</t>
+  </si>
+  <si>
+    <t>Get-ExecutionPolicy</t>
+  </si>
+  <si>
+    <t>-List</t>
+  </si>
+  <si>
+    <t>Geeft een lijst weer van de executionpolicy voor elke scope</t>
+  </si>
+  <si>
+    <t>Variabelen</t>
+  </si>
+  <si>
+    <t>ForEach-Object, and Switch.</t>
+  </si>
+  <si>
+    <t>$^</t>
+  </si>
+  <si>
+    <t>This contains the first token of the last line input into the shell.</t>
+  </si>
+  <si>
+    <t>This contains the last token of the last line input into the shell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is the current pipeline object; it’s used in script blocks, filters, Where-Object, </t>
   </si>
 </sst>
 </file>
@@ -273,7 +321,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -288,6 +336,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -589,10 +638,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39:B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -864,6 +913,75 @@
       <c r="B26" s="5"/>
       <c r="C26" s="3" t="s">
         <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B38" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B39" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B40" s="3" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>